<commit_message>
AdminViewVoca 함수형 -> class형으로 변경
</commit_message>
<xml_diff>
--- a/main/DB/WordList.xlsx
+++ b/main/DB/WordList.xlsx
@@ -3068,7 +3068,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -3081,6 +3081,9 @@
     </xf>
     <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
@@ -3393,9 +3396,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="5" width="14.005" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="5" width="31.862142857142857" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="5" width="6.005" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="6" width="14.005" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="6" width="31.862142857142857" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="6" width="6.005" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
@@ -4828,14 +4831,14 @@
         <v>5</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="131" customHeight="1" ht="19.5">
-      <c r="A131" s="2" t="s">
+    <row x14ac:dyDescent="0.25" r="131" customHeight="1" ht="18">
+      <c r="A131" s="5" t="s">
         <v>990</v>
       </c>
-      <c r="B131" s="2" t="s">
+      <c r="B131" s="5" t="s">
         <v>991</v>
       </c>
-      <c r="C131" s="2" t="s">
+      <c r="C131" s="5" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>